<commit_message>
Fake user data added to templates.xslx
</commit_message>
<xml_diff>
--- a/etc/templates.xlsx
+++ b/etc/templates.xlsx
@@ -4,18 +4,19 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="22995" windowHeight="10035"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="22995" windowHeight="10035" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Template" sheetId="1" r:id="rId1"/>
     <sheet name="Points of interest" sheetId="2" r:id="rId2"/>
+    <sheet name="Fake Points - Florida" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="57">
   <si>
     <t>Name</t>
   </si>
@@ -162,6 +163,30 @@
   </si>
   <si>
     <t>Get a private tour of Hearst Castle right from your phone using the interactive map in the Hearst Castle mobile app. Listen to in-depth narration from Castle historians, view never before seen photos, and play popular music from the time.</t>
+  </si>
+  <si>
+    <t>instance</t>
+  </si>
+  <si>
+    <t>Lead User Latitude</t>
+  </si>
+  <si>
+    <t>User 2 Latitude</t>
+  </si>
+  <si>
+    <t>User 3 Latitude</t>
+  </si>
+  <si>
+    <t>User 2 Longitude</t>
+  </si>
+  <si>
+    <t>User 3 Longitude</t>
+  </si>
+  <si>
+    <t>*** User Three Encount Problem</t>
+  </si>
+  <si>
+    <t>*** Group decides to go to Juptier Island</t>
   </si>
 </sst>
 </file>
@@ -502,8 +527,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F4" sqref="F4:G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -632,7 +657,7 @@
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="D15" sqref="D15:E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -919,4 +944,403 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>29.9107507079447</v>
+      </c>
+      <c r="C2">
+        <v>-81.313592409669596</v>
+      </c>
+      <c r="D2">
+        <v>29.911420290532501</v>
+      </c>
+      <c r="E2">
+        <v>-81.312390780030796</v>
+      </c>
+      <c r="F2">
+        <v>29.9120898686188</v>
+      </c>
+      <c r="G2">
+        <v>-81.311704134522699</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>29.835431168878301</v>
+      </c>
+      <c r="C3">
+        <v>-81.320716356812696</v>
+      </c>
+      <c r="D3">
+        <v>29.842578546534899</v>
+      </c>
+      <c r="E3">
+        <v>-81.322089647828804</v>
+      </c>
+      <c r="F3">
+        <v>29.847343180827899</v>
+      </c>
+      <c r="G3">
+        <v>-81.323462938844003</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>29.549714853149499</v>
+      </c>
+      <c r="C4">
+        <v>-81.285010790406304</v>
+      </c>
+      <c r="D4">
+        <v>29.577188399379398</v>
+      </c>
+      <c r="E4">
+        <v>-81.286384081421403</v>
+      </c>
+      <c r="F4">
+        <v>29.610624366493902</v>
+      </c>
+      <c r="G4">
+        <v>-81.291877245484002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>29.345221060567901</v>
+      </c>
+      <c r="C5">
+        <v>-81.149054979859002</v>
+      </c>
+      <c r="D5">
+        <v>29.355994157883099</v>
+      </c>
+      <c r="E5">
+        <v>-81.162787890015295</v>
+      </c>
+      <c r="F5">
+        <v>29.365569288019799</v>
+      </c>
+      <c r="G5">
+        <v>-81.172400927125196</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>29.152317645156401</v>
+      </c>
+      <c r="C6">
+        <v>-81.0666575189219</v>
+      </c>
+      <c r="D6">
+        <v>29.195484563183001</v>
+      </c>
+      <c r="E6">
+        <v>-81.088630175171104</v>
+      </c>
+      <c r="F6">
+        <v>29.219458336307099</v>
+      </c>
+      <c r="G6">
+        <v>-81.105109667358704</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>28.830394634201799</v>
+      </c>
+      <c r="C7">
+        <v>-80.907355761109301</v>
+      </c>
+      <c r="D7">
+        <v>28.859264379655301</v>
+      </c>
+      <c r="E7">
+        <v>-80.9183420892344</v>
+      </c>
+      <c r="F7">
+        <v>29.113931815349002</v>
+      </c>
+      <c r="G7">
+        <v>-81.039191698609201</v>
+      </c>
+      <c r="I7" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>28.830394634201799</v>
+      </c>
+      <c r="C8">
+        <v>-80.907355761109301</v>
+      </c>
+      <c r="D8">
+        <v>28.859264379655301</v>
+      </c>
+      <c r="E8">
+        <v>-80.9183420892344</v>
+      </c>
+      <c r="F8">
+        <v>28.883316378915101</v>
+      </c>
+      <c r="G8">
+        <v>-80.9293284173595</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>28.459190425189401</v>
+      </c>
+      <c r="C9">
+        <v>-80.830451464232993</v>
+      </c>
+      <c r="D9">
+        <v>28.386725332899601</v>
+      </c>
+      <c r="E9">
+        <v>-80.802985643921204</v>
+      </c>
+      <c r="F9">
+        <v>28.4495312793991</v>
+      </c>
+      <c r="G9">
+        <v>-80.813971972046303</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>28.106061397387599</v>
+      </c>
+      <c r="C10">
+        <v>-80.709601854858093</v>
+      </c>
+      <c r="D10">
+        <v>28.183559669324701</v>
+      </c>
+      <c r="E10">
+        <v>-80.715095018920707</v>
+      </c>
+      <c r="F10">
+        <v>28.193243008970502</v>
+      </c>
+      <c r="G10">
+        <v>-80.709601854858093</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>27.4304486507646</v>
+      </c>
+      <c r="C11">
+        <v>-80.407477831420593</v>
+      </c>
+      <c r="D11">
+        <v>27.5279169782251</v>
+      </c>
+      <c r="E11">
+        <v>-80.456916307983406</v>
+      </c>
+      <c r="F11">
+        <v>27.557140649474899</v>
+      </c>
+      <c r="G11">
+        <v>-80.489875292358604</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>27.163799994017499</v>
+      </c>
+      <c r="C12">
+        <v>-80.305854296263703</v>
+      </c>
+      <c r="D12">
+        <v>27.190676883070701</v>
+      </c>
+      <c r="E12">
+        <v>-80.327826952513902</v>
+      </c>
+      <c r="F12">
+        <v>27.215104799611002</v>
+      </c>
+      <c r="G12">
+        <v>-80.344306444701502</v>
+      </c>
+      <c r="I12" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>27.0562277718441</v>
+      </c>
+      <c r="C13">
+        <v>-80.121833300169797</v>
+      </c>
+      <c r="D13">
+        <v>27.063565524779001</v>
+      </c>
+      <c r="E13">
+        <v>-80.116340136108093</v>
+      </c>
+      <c r="F13">
+        <v>27.0684570933517</v>
+      </c>
+      <c r="G13">
+        <v>-80.1135935540768</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>26.999955725568999</v>
+      </c>
+      <c r="C14">
+        <v>-80.091620897826701</v>
+      </c>
+      <c r="D14">
+        <v>27.034211633332699</v>
+      </c>
+      <c r="E14">
+        <v>-80.105353807983093</v>
+      </c>
+      <c r="F14">
+        <v>27.0684570933517</v>
+      </c>
+      <c r="G14">
+        <v>-80.1135935540768</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <v>26.952224746152101</v>
+      </c>
+      <c r="C15">
+        <v>-80.090247606811502</v>
+      </c>
+      <c r="D15">
+        <v>26.984047648061001</v>
+      </c>
+      <c r="E15">
+        <v>-80.094367479857993</v>
+      </c>
+      <c r="F15">
+        <v>26.977928557744999</v>
+      </c>
+      <c r="G15">
+        <v>-80.091620897826701</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>